<commit_message>
se agrego datos a firmas, se arregla navbar
</commit_message>
<xml_diff>
--- a/certificado/static/docs/aulaTaller_Original.xlsx
+++ b/certificado/static/docs/aulaTaller_Original.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -55,10 +55,16 @@
     <t xml:space="preserve">Puesto Iz</t>
   </si>
   <si>
+    <t xml:space="preserve">Abajo Iz</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nombre D</t>
   </si>
   <si>
     <t xml:space="preserve">Puesto D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abajo D</t>
   </si>
 </sst>
 </file>
@@ -159,13 +165,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3"/>
+      <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -206,6 +212,12 @@
       </c>
       <c r="M1" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>